<commit_message>
Making ExcelDataProvider independent of row order
- Removes the hard dependency the excel column data has with the order
  of fields declared on the Data Object. However, the field names
  should exactly match the column data.
</commit_message>
<xml_diff>
--- a/dataproviders/src/test/resources/User.xlsx
+++ b/dataproviders/src/test/resources/User.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24030"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16120" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="USER" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="91">
   <si>
     <t>rama</t>
   </si>
@@ -40,9 +40,6 @@
     <t>suri</t>
   </si>
   <si>
-    <t>sStreet</t>
-  </si>
-  <si>
     <t>ph1</t>
   </si>
   <si>
@@ -79,9 +76,6 @@
     <t>123 Hyatt st</t>
   </si>
   <si>
-    <t>rcAddress</t>
-  </si>
-  <si>
     <t>bnk2</t>
   </si>
   <si>
@@ -151,24 +145,9 @@
     <t>1-213-580-6070</t>
   </si>
   <si>
-    <t>lrcAreaCode</t>
-  </si>
-  <si>
     <t>sKey</t>
   </si>
   <si>
-    <t>sName</t>
-  </si>
-  <si>
-    <t>sPassword</t>
-  </si>
-  <si>
-    <t>lAccountNumber</t>
-  </si>
-  <si>
-    <t>dAmount</t>
-  </si>
-  <si>
     <t>100.00</t>
   </si>
   <si>
@@ -178,18 +157,6 @@
     <t>300.75</t>
   </si>
   <si>
-    <t>rcBank</t>
-  </si>
-  <si>
-    <t>sPhoneNumber</t>
-  </si>
-  <si>
-    <t>sType</t>
-  </si>
-  <si>
-    <t>sAreaCode</t>
-  </si>
-  <si>
     <t>preintTest</t>
   </si>
   <si>
@@ -202,18 +169,12 @@
     <t>17</t>
   </si>
   <si>
-    <t>boolean</t>
-  </si>
-  <si>
     <t>true</t>
   </si>
   <si>
     <t>false</t>
   </si>
   <si>
-    <t>double</t>
-  </si>
-  <si>
     <t>12.5</t>
   </si>
   <si>
@@ -223,9 +184,6 @@
     <t>14.5</t>
   </si>
   <si>
-    <t>long</t>
-  </si>
-  <si>
     <t>167045</t>
   </si>
   <si>
@@ -235,12 +193,6 @@
     <t>456567</t>
   </si>
   <si>
-    <t>float</t>
-  </si>
-  <si>
-    <t>byte</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
@@ -299,6 +251,51 @@
   </si>
   <si>
     <t>SkipMeAsWell</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>areaCode</t>
+  </si>
+  <si>
+    <t>bank</t>
+  </si>
+  <si>
+    <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>isbooleanGood</t>
+  </si>
+  <si>
+    <t>doubleTest</t>
+  </si>
+  <si>
+    <t>longTest</t>
+  </si>
+  <si>
+    <t>byteTest</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>street</t>
+  </si>
+  <si>
+    <t>floattest</t>
+  </si>
+  <si>
+    <t>accountnumber</t>
+  </si>
+  <si>
+    <t>PASSWORD</t>
   </si>
 </sst>
 </file>
@@ -660,113 +657,113 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.1640625" style="1"/>
-    <col min="3" max="3" width="11.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="11.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="13" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1640625" style="1"/>
+    <col min="8" max="8" width="16.42578125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="J1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="C2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="L2" s="1" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -775,40 +772,40 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="K3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -819,42 +816,42 @@
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
@@ -863,42 +860,42 @@
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
@@ -907,37 +904,37 @@
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N7" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -956,57 +953,57 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="1"/>
-    <col min="2" max="3" width="13.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="3" width="13.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1024,68 +1021,68 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1107,43 +1104,43 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="12.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1160,34 +1157,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>